<commit_message>
tacMaster 90% without test
</commit_message>
<xml_diff>
--- a/src/main/resources/data/transactions.xlsx
+++ b/src/main/resources/data/transactions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Transaction Id</t>
   </si>
@@ -38,6 +38,27 @@
   </si>
   <si>
     <t>Customer New Balance</t>
+  </si>
+  <si>
+    <t>ab445aa0-8f60-4ed3-b2c3-120b767cbc3e</t>
+  </si>
+  <si>
+    <t>443c417b-e01e-404c-a964-27f3671840fa</t>
+  </si>
+  <si>
+    <t>ogya test</t>
+  </si>
+  <si>
+    <t>SAMSUNG, XIAOMI</t>
+  </si>
+  <si>
+    <t>2300.00</t>
+  </si>
+  <si>
+    <t>700.00</t>
+  </si>
+  <si>
+    <t>3000.00</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1058,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H6" sqref="A2:H6"/>
@@ -1045,14 +1066,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="12.8583333333333" customWidth="1"/>
-    <col min="2" max="2" width="20.8583333333333" customWidth="1"/>
-    <col min="3" max="3" width="14.8583333333333" customWidth="1"/>
-    <col min="4" max="4" width="13.7083333333333" customWidth="1"/>
-    <col min="5" max="5" width="16.2833333333333" customWidth="1"/>
-    <col min="6" max="6" width="9.425" customWidth="1"/>
-    <col min="7" max="7" width="20.1416666666667" customWidth="1"/>
-    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="12.8583333333333"/>
+    <col min="2" max="2" customWidth="true" width="20.8583333333333"/>
+    <col min="3" max="3" customWidth="true" width="14.8583333333333"/>
+    <col min="4" max="4" customWidth="true" width="13.7083333333333"/>
+    <col min="5" max="5" customWidth="true" width="16.2833333333333"/>
+    <col min="6" max="6" customWidth="true" width="9.425"/>
+    <col min="7" max="7" customWidth="true" width="20.1416666666667"/>
+    <col min="8" max="8" customWidth="true" width="21.0"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" spans="1:8">
@@ -1079,6 +1100,32 @@
       </c>
       <c r="H1" s="3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>